<commit_message>
feat: Introduce INSIGHT tool with Flask webhook handling, LangGraph-based bug localization workflow, and evaluation utilities.
</commit_message>
<xml_diff>
--- a/Replication Package/Evaluation/test_dataset.xlsx
+++ b/Replication Package/Evaluation/test_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2782,6 +2782,4423 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>132</v>
+      </c>
+      <c r="E32" t="n">
+        <v>15</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Fail result for `Flags and flag attributes` check with no reasoning</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Running the CF checker on [this file](http://thredds.aodn.org.au/thredds/fileServer/IMOS/SRS/SST/ghrsst/L3S-1d/dn/2016/20160919092000-ABOM-L3S_GHRSST-SSTfnd-AVHRR_D-1d_dn.nc) results in 
+```
+Name                             Priority:     Score:Reasoning
+--------------------------------------------------------------------------------
+§3.5 Flags and flag attributes         :3:    31/32 :  
+```
+An apparently failed result, with no reasoning message.
+</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/316</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/cf.py']</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>['CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>[929, 930, 932, 935, 936, 937]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/362d8a38bec497487ade40140b536a5756adbc71...44bcd8580f13d03762762eacd1664321c31d7274</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>132</v>
+      </c>
+      <c r="E33" t="n">
+        <v>15</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>CF Checker records omission of “reference” global attribute as an error</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Originally part of #501
+(8) IOOS checker records omission of “reference” global attribute as an error: use of this attribute is neither required nor recommended.</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/510</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/cf.py', 'compliance_checker/tests/test_cf.py']</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>['TestCF', 'CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>[803, 804, 250, 259]</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/5b0830c466a3cec9e71677c193bf64fe3634adcf...b827a8288d4f975eb570d6af5c1c7c5bcdf882c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>132</v>
+      </c>
+      <c r="E34" t="n">
+        <v>15</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>JSON output issue in 3.0.3 with ERDDAP URLs</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>I've been testing the new Compliance Checker release with ERDDAP (on Windows), and I see some different results in the output when using ERDDAP URLs with the JSON output format than OPeNDAP.
+I made a test script that illustrates the issue: https://gist.github.com/mwengren/68f61b0e70868a57336b81f863d7dbc9
+Or, I think you can see the same issue (in my environment at least) by running these commands:
+```
+compliance-checker -t cf -f json http://coastwatch.pfeg.noaa.gov/erddap/griddap/osuSstAnom
+compliance-checker -t cf -f json http://ona.coas.oregonstate.edu:8080/thredds/dodsC/NANOOS/OCOS
+```
+The issue is that when I try to hit the ERDDAP URL, it includes what looks like a debug line in stdout:
+```
+Using cached standard name table v29 from C:\\Users\\Micah.Wengren\\.local\\share\\compliance-checker\\cf-standard-name-table-test-29.xml
+{
+  "cf": {
+    "scored_points": 168,
+    "low_count": 0,
+...
+```
+When I try to parse this into JSON using subprocess.Popen (see the Gist), if fails because it can't parse the first line. 
+I'm using 3.0.3:
+```
+$ compliance-checker --version
+IOOS compliance checker version 3.0.3
+```
+Also, not sure if it matters, but I'm using Python 2.7 for these tests.</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/497</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/util.py', 'compliance_checker/cf/cf.py']</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>['download_cf_standard_name_table', 'CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>[3, 14, 136, 146, 148, 154, 1, 6, 332]</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/66ec69eaab33a56aedbf116487867170f5228afc...4e3c9f05d69122b3e038db7c999d44fea8f65ef3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>132</v>
+      </c>
+      <c r="E35" t="n">
+        <v>15</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>CFBaseCheck::check_cell_measures() failing</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi,
+There are 2 small bugs in the CF suite (`check_cell_measure()` method), which eluded detection because corresponding [unit test](https://github.com/ioos/compliance-checker/blob/master/compliance_checker/tests/test_cf.py#L352) doesn't really test the right thing.
+1. netcdf4's [get_variables_by_attributes](https://github.com/ioos/compliance-checker/blob/master/compliance_checker/cf/cf.py#L2579) returns a list of variables, not just their names, so they cannot be used for indexing of ds.variables
+Something along these lines should fix it
+```python
+tested_vars = ds.get_variables_by_attributes(cell_measures=lambda c: c is not None)
+for tested_var in tested_vars:
+    var_name = tested_var.name
+        var = ds.variables[var_name]
+```
+2. Also, a few lines below, `search_res.groups[0]` will fail because `groups` in `re.MatchObject` is a method, not an attribute (unlike in `re.RegexObject`)
+</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/495</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/cf.py']</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>['CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>[2599, 2600, 2601, 2602, 2605, 2606, 2607, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2627, 2628, 2629, 2630, 2631]</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/8c3010faedf38dd1a0bd61f5f8803a3fee107d64...621369608f70a8b60b5cec2029fa8a0e83ea4972</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>132</v>
+      </c>
+      <c r="E36" t="n">
+        <v>15</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>ACDD checks for "acknowledgement", IOOS checks for "acknowledgment"</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>When running "cchecker.py -t acdd:latest", it looks for either "acknowledgment" (US spelling, from deprecated UDDC convention) or "acknowledgement" (UK spelling, as required by superceding ACDD convention). However, when running "cchecker.py -t ioos:latest", the test only looks for the deprecated US spelling. It should either look for both spellings like the ACDD test or switch to the UK spelling as currently required.
+Example:
+http://www.pacioos.hawaii.edu/archive/WQB04agg/WQB04agg.2010.nc
+Snippet for cchecker.py output:
+Platform Sponsor                       :3:     0/ 1 : Attr 'acknowledgment'
+                                                      (IOOS concept: 'Platform
+                                                      Sponsor') not found in
+                                                      dataset</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/465</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>['compliance_checker/ioos.py']</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>['IOOSNCCheck']</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>[55]</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/cef261facf389df506599026e1f74ed0e1887fe0...39a08583e73fc0caf05959148b903be945b6a22b</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>132</v>
+      </c>
+      <c r="E37" t="n">
+        <v>15</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>CDL check fails on text files (py3)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The recent CDL additions (#297) have broken the ability to pass a text file on the command line (IE a getcaps/describesensor xml document) on python 3 environments:
+```
+~/dev/compliance-checker -&gt; python cchecker.py --test ioos ~/Downloads/aoos_sos_getcaps.xml
+Running Compliance Checker on the dataset from: /home/daf/Downloads/aoos_sos_getcaps.xml
+Traceback (most recent call last):
+  File "cchecker.py", line 79, in &lt;module&gt;
+    sys.exit(main())
+  File "cchecker.py", line 68, in main
+    args.format)
+  File "/home/daf/dev/compliance-checker/compliance_checker/runner.py", line 44, in run_checker
+    ds = cs.load_dataset(ds_loc)
+  File "/home/daf/dev/compliance-checker/compliance_checker/suite.py", line 576, in load_dataset
+    elif is_cdl_file(ds_str, first_chunk):
+  File "/home/daf/dev/compliance-checker/compliance_checker/suite.py", line 567, in is_cdl_file
+    if data.startswith('netcdf') or 'dimensions' in data:
+TypeError: startswith first arg must be bytes or a tuple of bytes, not str
+```
+</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/308</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>['compliance_checker/suite.py']</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>['CheckSuite']</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>[485, 487, 527, 567, 580]</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/437b4c8c1dbd3f2630cfbdfe1eee90bcbbc3f548...79119cc53226d4ff4c54a54329e56212876852c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>132</v>
+      </c>
+      <c r="E38" t="n">
+        <v>15</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Save text output</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">@lukecampbell and @daf I am helping @jbosch-noaa with some notebooks in
+https://github.com/ioos/notebooks_demos/pull/21
+and I noticed that simple text outputs are only redirected to `stdout`. There is on API to save it to a file.
+Correct me if I am wrong but I could not see it [here](https://github.com/ioos/compliance-checker/blob/7276abba102e2ef6cb390d49ba0c38726f625913/compliance_checker/runner.py#L43-L50).
+I do know that in CLI interface it is easy to redirect to a file but it would be nice to be able to do that from class method too. Not also that the docs give the idea that this is possible and the error message [here](https://github.com/ioos/compliance-checker/blob/7276abba102e2ef6cb390d49ba0c38726f625913/compliance_checker/runner.py#L53) is not very helpful.
+</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/290</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>['compliance_checker/tests/test_cli.py', 'compliance_checker/runner.py']</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>['TestCLI', 'ComplianceChecker']</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>[7, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 89, 112, 135, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114]</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/9a453b86ebb32dcdd4826d57eb5d9cdff908186f...c625d0f9cf41d55f03b05bbb0dcb9bb68f991734</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>132</v>
+      </c>
+      <c r="E39" t="n">
+        <v>15</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>JSON output missing argument</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Attempting to run compliance-checker on Python 2 or 3 with JSON output fails due to a missing function argument.
+```
+compliance-checker --test ioos -f json -c strict compliance_checker/tests/data/conv_bad.nc                                                                    
+Traceback (most recent call last):
+  File "/home/badams_local/.virtualenvs/cchecker_py3/bin/compliance-checker", line 9, in &lt;module&gt;
+    load_entry_point('compliance-checker', 'console_scripts', 'compliance-checker')()
+  File "/home/badams_local/devel/compliance-checker/cchecker.py", line 41, in main
+    args.format)
+  File "/home/badams_local/devel/compliance-checker/compliance_checker/runner.py", line 50, in run_checker
+    groups = cls.json_output(cs, score_groups, output_filename, ds_loc, limit)
+  File "/home/badams_local/devel/compliance-checker/compliance_checker/runner.py", line 116, in json_output
+    cs.json_output(checker, groups, f, ds_loc)
+TypeError: json_output() missing 1 required positional argument: 'limit'
+```
+</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/255</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>['compliance_checker/tests/test_cli.py', 'compliance_checker/suite.py']</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>['CheckSuite', 'TestCLI']</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>[228, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93]</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/34e8283479135a96b7aa4e03e91cce0617e9fac2...7f9da67575306c1c92d3b23ccd3eaf1ded6fa662</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>132</v>
+      </c>
+      <c r="E40" t="n">
+        <v>15</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Question about data type for flag_masks</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about the data type allowed for a flag_masks variable.
+See CF.py code 
+``` python
+        type_ok = v.dtype in [np.character,
+                                      np.dtype('b'),
+                                      np.dtype('i4'),
+                                      np.int32]
+```
+https://github.com/ioos/compliance-checker/blob/master/compliance_checker/cf/cf.py#L811
+is there a reason why int8 and int32 are allowed and int16 is not. I previously had a file
+with a flag_masks variable of "short' type not passing the CF checker
+Thanks
+@mhidas FYI
+</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/196</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/cf.py']</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>['CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>[857, 858, 859]</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/e5a8f37215f7d5eb749ccd231a01d844d3bdffe3...8a6a520a2243959637a80e7162112ea674b7eb5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>132</v>
+      </c>
+      <c r="E41" t="n">
+        <v>15</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Test "dimension_order" with inconsistent results</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This [file](http://thredds.aodn.org.au/thredds/catalog/IMOS/eMII/checker_test/ANMN/timeSeriesProfile/catalog.html?dataset=eMII/checker_test/ANMN/timeSeriesProfile/IMOS_ANMN-QLD_AETVZ_20110307T111900Z_GBRHIS_FV00_GBRHIS-1103-Workhorse-ADCP-model-Sentinel-or-Monitor-44_END-20110813T105900Z_C-20160203T040408Z.nc) and this [one](http://thredds.aodn.org.au/thredds/catalog/IMOS/eMII/checker_test/ANMN/timeSeriesProfile/catalog.html?dataset=eMII/checker_test/ANMN/timeSeriesProfile/IMOS_ANMN-QLD_AETVZ_20110307T111900Z_GBRHIS_FV01_GBRHIS-1103-Workhorse-ADCP-model-Sentinel-or-Monitor-44_END-20110813T105900Z_C-20160203T040408Z.nc) both include VCUR or VCUR_MAG such as:
+```
+float VCUR(TIME, HEIGHT_ABOVE_SENSOR) ;
+                VCUR:coordinates = "TIME LATITUDE LONGITUDE HEIGHT_ABOVE_SENSOR" ;
+                VCUR:standard_name = "northward_sea_water_velocity" ;
+                VCUR:long_name = "northward_sea_water_velocity" ;
+                VCUR:units = "m s-1" ;
+                VCUR:valid_min = -10.f ;
+                VCUR:valid_max = 10.f ;
+                VCUR:_FillValue = 999999.f ;
+                VCUR:comment = "magneticDeclinationPP: data initially referring to magnetic North has been modified so that it now refers to true North, applying a computed magnetic declination of 9.7degrees. NOAA\\'s Geomag v7.0 software + IGRF12 model have been used to compute this value at a latitude=-23.5136degrees North, longitude=151.9553degrees East, depth=44m (instrument nominal depth) and date=2011/05/25 (date in the middle of time_coverage_start and time_coverage_end)." ;
+                VCUR:ancillary_variables = "VCUR_quality_control" ;
+                VCUR:magnetic_declination = 9.7 ;
+                VCUR:compass_correction_applied = 9.7 ;
+```
+with
+```
+double TIME(TIME) ;
+        TIME:standard_name = "time" ;
+        TIME:long_name = "time" ;
+        TIME:units = "days since 1950-01-01 00:00:00 UTC" ;
+        TIME:calendar = "gregorian" ;
+        TIME:axis = "T" ;
+        TIME:valid_min = 0. ;
+        TIME:valid_max = 90000. ;
+```
+and
+```
+float HEIGHT_ABOVE_SENSOR(HEIGHT_ABOVE_SENSOR) ;
+        HEIGHT_ABOVE_SENSOR:comment = "Data has been vertically bin-mapped using tilt information so that the cells have consistant heights above sensor in time." ;
+        HEIGHT_ABOVE_SENSOR:long_name = "height_above_sensor" ;
+        HEIGHT_ABOVE_SENSOR:units = "m" ;
+        HEIGHT_ABOVE_SENSOR:axis = "Z" ;
+        HEIGHT_ABOVE_SENSOR:positive = "up" ;
+        HEIGHT_ABOVE_SENSOR:reference_datum = "sensor" ;
+        HEIGHT_ABOVE_SENSOR:valid_min = -12000.f ;
+        HEIGHT_ABOVE_SENSOR:valid_max = 12000.f 
+```
+However the first one passes the cf check while the second fails on the dimension_order test:
+```
+dimension_order                        :1:    82/126 : Variable VCUR has a non-
+                                                      space-time dimension after
+                                                      space-time-dimensions
+```
+And I don't think this message should output since HEIGHT_ABOVE_SENSOR is a space dimension.
+</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/issues/200</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>['compliance_checker/cf/cf.py']</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>['CFBaseCheck']</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>[409, 410, 411, 412, 413]</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>https://github.com/ioos/compliance-checker/compare/39c3c90fe8174b05f544625413915a7f63e8250e...b51f940d0b053918cb99cfbc1cacc781cf43afad</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>113</v>
+      </c>
+      <c r="E42" t="n">
+        <v>21</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Test suite hangs if it can't connect to the specified API</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>A global fallback timeout for requests should be included in case of this sort of error condition.</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/85</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>['IS0401Test.py', 'IS05Utils.py', 'Config.py', 'TestHelper.py', 'IS0501Test.py']</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>['IS0401Test', 'do_request', 'IS05Utils', 'IS0501Test']</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>[34, 35, 36, 201, 202, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 827, 828, 834, 835, 560, 561, 572, 573, 584, 585, 591, 19, 20, 23, 24, 50, 61]</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/5b38d2ce134d571c2c89ee8f1a5c82fd5efb68cd...d6fd93692aa277963858cce36caffc6d18ccd83b</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>113</v>
+      </c>
+      <c r="E43" t="n">
+        <v>21</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>IS-05 "Interaction with Node API" independence of tests</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Considering that the uninitialized state of a sender or receiver resource will return "auto" as value for the destination port when doing a GET on the staged parameters, tests 7, 8, 9, 10 and 11 will fail if tested individually and in a uninitialized state. This is the case since in IS0502Test.py, the activate_check_parked function will do a GET on the staged and the active parameters and compare the destination ports to make sure they are identical. This will inevitably fail, unless tests 5 and 6 are executed prior to these tests (or the value of the destination port in the staged parameters was already modified to something other than auto and applied to the active parameters before this test) since the tests 5 and 6 will modify the destination port and make sure the value is different than auto.
+Ideally these tests should not depend on the state of the staged parameters and should make sure to modify the destination port in the staged parameters, and apply the settings to the active parameters, before comparing the staged and active values.
+Not critical, but it could cause confusion when trying to debug an individual test case. :^)</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/116</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>['IS05Utils.py']</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>['IS05Utils']</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>[122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 136, 212, 295, 610, 611, 641, 642]</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/34cd48a45db0147b1a85ede2e2308182e8590ab6...cacad52b1975cbdc8eba2b317aec0195b7bbacbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>113</v>
+      </c>
+      <c r="E44" t="n">
+        <v>21</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>IS-04-01 test_21 the mock registry does not return location header</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>During test_21, the mock registry returns a HTTP 200 when trying to register, the node should then perform a DELETE using the location header in the response, but the header is missing from the 200 response</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/396</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>['nmostesting/mocks/Registry.py']</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>['post_resource']</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>[141, 142, 144, 146]</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/7b4e75eb22256528cc7d58a4bb2d82339f66a011...820f023d4704dc8ae243bf1a7576639d887511b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>113</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>KeyError in IS0502 test for park resource test</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Line 604 of park_resource in IS05_Utils, when a response fails to include the 'transport_params' key in its response.
+May indicate a need for a more general catching of KeyErrors to ensure a 'FAIL' is presented rather than a traceback.
+```
+ * Running test_07_rx_nmos_updates_sub
+ * ERROR: 'transport_params'
+192.168.200.24 - - [15/Jan/2019 14:30:35] "POST / HTTP/1.1" 500 -
+Traceback (most recent call last):
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2309, in __call__
+    return self.wsgi_app(environ, start_response)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2295, in wsgi_app
+    response = self.handle_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1741, in handle_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2292, in wsgi_app
+    response = self.full_dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1815, in full_dispatch_request
+    rv = self.handle_user_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1718, in handle_user_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1813, in full_dispatch_request
+    rv = self.dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1799, in dispatch_request
+    return self.view_functions[rule.endpoint](**req.view_args)
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 218, in index_page
+    raise ex
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 215, in index_page
+    result = test_obj.run_tests(test_selection)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 133, in run_tests
+    self.execute_tests(test_name)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 101, in execute_tests
+    self.result.append(method())
+  File "/home/ipstudio-admin/nmos-testing/IS0502Test.py", line 401, in test_07_rx_nmos_updates_sub
+    valid, response = self.activate_check_parked(resource_type)
+  File "/home/ipstudio-admin/nmos-testing/IS0502Test.py", line 161, in activate_check_parked
+    valid, response = self.is05_utils.park_resource(resource_type, is05_resource)
+  File "/home/ipstudio-admin/nmos-testing/IS05Utils.py", line 604, in park_resource
+    staged_params = response['transport_params']
+KeyError: 'transport_params'
+```</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/87</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>['GenericTest.py', 'IS05Utils.py']</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>['IS05Utils', 'GenericTest']</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[20, 105, 106, 117, 118, 119, 120, 121, 122, 123, 124, 125, 604, 605, 606, 607]</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/4670da31484d2bd1adbba507b925ba465dc467d5...98d87e794a00e859ebdf3284972485fa50d15dbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>113</v>
+      </c>
+      <c r="E46" t="n">
+        <v>21</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>IndexError list index out of range in IS0501Test</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>When running test_15, a failure was recorded on line 907 of IS0501Test.py in check_staged_complies_with_constraints
+```
+ * Running test_15
+ * ERROR: list index out of range
+192.168.201.184 - - [15/Jan/2019 15:01:55] "POST / HTTP/1.1" 500 -
+Traceback (most recent call last):
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2309, in __call__
+    return self.wsgi_app(environ, start_response)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2295, in wsgi_app
+    response = self.handle_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1741, in handle_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2292, in wsgi_app
+    response = self.full_dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1815, in full_dispatch_request
+    rv = self.handle_user_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1718, in handle_user_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1813, in full_dispatch_request
+    rv = self.dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1799, in dispatch_request
+    return self.view_functions[rule.endpoint](**req.view_args)
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 218, in index_page
+    raise ex
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 215, in index_page
+    result = test_obj.run_tests(test_selection)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 133, in run_tests
+    self.execute_tests(test_name)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 101, in execute_tests
+    self.result.append(method())
+  File "/home/ipstudio-admin/nmos-testing/IS0501Test.py", line 383, in test_15
+    valid, response = self.check_staged_complies_with_constraints("sender", self.senders)
+  File "/home/ipstudio-admin/nmos-testing/IS0501Test.py", line 907, in check_staged_complies_with_constraints
+    schema.update(constraints_response[count])
+IndexError: list index out of range
+```</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/88</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>['IS0501Test.py']</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>['IS0501Test']</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>[907, 908, 909, 910, 911]</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/4670da31484d2bd1adbba507b925ba465dc467d5...bbe59772767784aa3aa8708c9e9d8ccea19c70ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>113</v>
+      </c>
+      <c r="E47" t="n">
+        <v>21</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>TypeError in IS0401Test test_13</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>String indices must be integers on line 359 test_13, where stream_type is identified.
+```
+ * Running test_13
+ * ERROR: string indices must be integers
+192.168.200.43 - - [15/Jan/2019 11:36:20] "POST / HTTP/1.1" 500 -
+Traceback (most recent call last):
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2309, in __call__
+    return self.wsgi_app(environ, start_response)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2295, in wsgi_app
+    response = self.handle_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1741, in handle_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 2292, in wsgi_app
+    response = self.full_dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1815, in full_dispatch_request
+    rv = self.handle_user_exception(e)
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1718, in handle_user_exception
+    reraise(exc_type, exc_value, tb)
+  File "/usr/local/lib/python3.5/dist-packages/flask/_compat.py", line 35, in reraise
+    raise value
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1813, in full_dispatch_request
+    rv = self.dispatch_request()
+  File "/usr/local/lib/python3.5/dist-packages/flask/app.py", line 1799, in dispatch_request
+    return self.view_functions[rule.endpoint](**req.view_args)
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 218, in index_page
+    raise ex
+  File "/home/ipstudio-admin/nmos-testing/nmos-test.py", line 215, in index_page
+    result = test_obj.run_tests(test_selection)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 133, in run_tests
+    self.execute_tests(test_name)
+  File "/home/ipstudio-admin/nmos-testing/GenericTest.py", line 101, in execute_tests
+    self.result.append(method())
+  File "/home/ipstudio-admin/nmos-testing/IS0401Test.py", line 359, in test_13
+    stream_type = receiver["format"].split(":")[-1]
+TypeError: string indices must be integers
+```</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/89</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>['IS0401Test.py']</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>['IS0401Test']</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>[359, 360, 361, 362, 363]</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/4670da31484d2bd1adbba507b925ba465dc467d5...309254eafb0abe84a716505a2f82cefcab51cc7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>113</v>
+      </c>
+      <c r="E48" t="n">
+        <v>21</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>MdnsListener has no attribute remove_service</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>AttributeError when using zeroconf mDNS.
+```
+ * Running test_13
+Exception in thread zeroconf-ServiceBrowser__nmos-node._tcp.local.:
+Traceback (most recent call last):
+  File "/usr/lib/python3.5/threading.py", line 914, in _bootstrap_inner
+    self.run()
+  File "/usr/local/lib/python3.5/dist-packages/zeroconf.py", line 1382, in run
+    handler(self.zc)
+  File "/usr/local/lib/python3.5/dist-packages/zeroconf.py", line 1329, in &lt;lambda&gt;
+    state_change=state_change,
+  File "/usr/local/lib/python3.5/dist-packages/zeroconf.py", line 1235, in fire
+    h(**kwargs)
+  File "/usr/local/lib/python3.5/dist-packages/zeroconf.py", line 1304, in on_change
+    listener.remove_service(*args)
+AttributeError: 'MdnsListener' object has no attribute 'remove_service'
+```</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/90</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>['MdnsListener.py']</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>['MdnsListener']</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>[33, 34, 35]</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/4670da31484d2bd1adbba507b925ba465dc467d5...7d27633e998ad605a00d867afe8799763a2f0b9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>113</v>
+      </c>
+      <c r="E49" t="n">
+        <v>21</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Automatic tests do not support sub-resources in channel mapping spec</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>The channel mapping /activations resource uses a new key/value pair format, with sub-resources accessed via a GET to /activations/{key}. The test suite doesn't support this format yet.</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/82</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>['GenericTest.py']</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>['GenericTest']</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>[321, 322, 323, 324, 325]</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/cd34fd20730a6319e16279ebf4bae45631cb4951...1384c45aefdc7b4886d40c4f150dcbd49a7fbe63</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>113</v>
+      </c>
+      <c r="E50" t="n">
+        <v>21</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Git clone fails if a remote branch has been deleted</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>When a v1.x-dev branch gets deleted, if you previously had it in your local cache of the spec files, the next git pull will fail. The only solution to this at present is to manually delete the cache directory. Ideally this should be detected and handled more gracefully.</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/75</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>['nmos-test.py']</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>[262, 263, 264, 265, 266, 267]</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/cd34fd20730a6319e16279ebf4bae45631cb4951...021c0cf5285dfb0c941760b8deea0bc34ed4b7fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>113</v>
+      </c>
+      <c r="E51" t="n">
+        <v>21</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Ramlfications fails to parse IS-07 global types</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>The IS-07 spec appears to use valid RAML 1.0, but ramlfications (being a 0.8 library) can't quite handle the way they're written. As such several tests appear as 'manual' when they should work.</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>https://github.com/AMWA-TV/nmos-testing/issues/78</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>['Specification.py']</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>['Specification']</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>[63, 66, 70, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 83, 85, 87, 89, 90, 91, 92, 93, 94, 95, 96]</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>https://github.com/amwa-tv/nmos-testing/compare/cd34fd20730a6319e16279ebf4bae45631cb4951...4c500bba1713a0d5dee270b176b97eb81f125604</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>138</v>
+      </c>
+      <c r="E52" t="n">
+        <v>22</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Environment variables do not get passed to subprocess during package building</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When Chalice creates subprocesses to build the package it does not pass down the current set of environment variables down. This was introduced in https://github.com/aws/chalice/commit/d6b22b3e8932dd588bf5110d5e5b084d246681a4 so it is a regression over the previous behavior where the subprocess inherited the environment. This matters for any setup.py file that makes use of an environment variable.
+Initial issue #497 </t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/501</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>['tests/functional/test_package.py', 'chalice/deploy/packager.py', 'tests/unit/deploy/test_packager.py', 'chalice/compat.py', 'chalice/utils.py']</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>['create_zip_file', 'TestPipRunner', 'FakePip', 'DependencyBuilder', 'SDistMetadataFetcher', 'PipRunner', 'SubprocessPip', 'osutils', 'TestSubprocessPip']</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>[11, 25, 266, 579, 580, 581, 582, 583, 584, 586, 588, 605, 606, 607, 608, 610, 613, 624, 13, 82, 83, 84, 85, 57, 166, 167, 168, 169, 170, 171, 172, 173, 174, 176, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 164, 173, 174, 177, 180, 189, 190, 193, 196, 206, 209, 225, 226, 230, 231, 239, 240, 246, 247]</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/a36ad3f9b413979da9416e1dec164bf787c7c0bf...5784fae3602227ba549b104e5803237180e611a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>138</v>
+      </c>
+      <c r="E53" t="n">
+        <v>22</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Packager assumes wheel to be installed</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Took me a while to figure out why Chalice fails to build my deployment package properly in one environment, but not the other. Funnily enough while I was trying to pin all transitive dependencies :(
+Chalice appears to use [wheel](https://github.com/aws/chalice/blob/9fe9ddc0423acd202c7e3533b74d14691336d8f7/chalice/deploy/packager.py#L693) regardless of whether wheel is installed in the environment. Should wheel be a setup requirement? Or perhaps include a warning in the "Could not install dependencies..." message?
+```
+$ python -m venv v1
+$ source v1/bin/activate
+$ pip install chalice  # wheel not installed
+$ chalice new-project v1-test
+$ cd v1-test
+$ echo "markupsafe" &gt;&gt; requirements.txt
+$ chalice package out
+Creating deployment package.
+Could not install dependencies:
+markupsafe==1.0
+You will have to build these yourself and vendor them in
+the chalice vendor folder.
+Your deployment will continue but may not work correctly
+if missing dependencies are not present. For more information:
+http://chalice.readthedocs.io/en/latest/topics/packaging.html
+$ pip install wheel
+$ chalice package out       
+Creating deployment package.
+# Success!
+```</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/928</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>['setup.py']</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>[18, 19]</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/cb3059551da903accff7d91d710fc998adfc1289...9524f4536becd9a31ec69e66e1075efe70d276db</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>138</v>
+      </c>
+      <c r="E54" t="n">
+        <v>22</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Fail to analyze list comprehension code</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chalice does not deploy below code with error message 'key_name'.
+If I change the code from item['payload'][key_name] to item['payload']['data'], it works well.
+I have used version 1.0.0b1.
+```python
+@app.route('/data/{node_name}', methods=['GET'], cors=True, authorizer=authorizer)
+def retrieve_data(node_name):
+    key_name = 'data'
+    response['Items'] = [
+        { 'Timestamp' : 10, 'payload' : { 'data' : 1}},
+        { 'Timestamp' : 11, 'payload' : { 'data' : 2}}
+    ]
+    stamp = [item['Timestamp'] for item in response['Items']]
+    temps = [item['payload'][key_name] for item in response['Items']]
+    hums = [item['payload'][key_name] for item in response['Items']]
+```
+</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/412</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>['tests/unit/test_analyzer.py', 'chalice/analyzer.py']</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>['test_can_handle_list_expr_with_api_calls', 'SymbolTableTypeInfer']</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>[568, 569, 581, 582, 585, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470]</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/69f18d739857983b90eebe4d292d93bb7f3a1b2b...bdee4eb1a263da680cb4286e6d992a7b815e9346</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>138</v>
+      </c>
+      <c r="E55" t="n">
+        <v>22</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Adding Content-Type to Response produced 2 Content-Type headers</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">`curl -v localhost:8000`
+`&gt;GET / HTTP/1.1`
+`&gt;Host: localhost:8000`
+`&gt;User-Agent: curl/7.52.1`
+` &gt;Accept: */*`
+` HTTP 1.0, assume close after body`
+`&lt; HTTP/1.0 200 OK`
+`&lt; Server: BaseHTTP/0.3 Python/2.7.12`
+`&lt; Date: Thu, 27 Apr 2017 20:30:54 GMT`
+`&lt; Content-Length: 83`
+`&lt; Content-Type: application/xml`
+`&lt; Content-Type: application/xml`
+`&lt; `
+` Curl_http_done: called premature == 0`
+` Closing connection 0`
+`&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;Response&gt;&lt;Say&gt;Hello World&lt;/Say&gt;`
+</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/310</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>['chalice/local.py', 'tests/unit/test_local.py']</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>['test_querystring_is_mapped', 'ChaliceRequestHandler', 'sample_app']</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>[123, 124, 125, 2, 70, 71, 72, 73, 74, 75, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206]</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/5bb2239abab06355da1fe4ef4ef2438ea3dd513a...173457ded8fd257b42c0f824e3c4af2290b71d14</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>138</v>
+      </c>
+      <c r="E56" t="n">
+        <v>22</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Setting app.debug does not propagate to app.log logger log level</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>In https://github.com/awslabs/chalice/blob/master/chalice/app.py#L434-L437, intent is shown to set the logger's log level according to the value of Chalice.debug. However, app.debug is currently hardcoded to false in `Chalice.__init__`, so without calling `Chalice. _configure_logging()` again or setting it manually via `app.log.setLevel(logging.DEBUG)`, it will always remain set to logging.ERROR.
+It would probably make more sense to have a `Chalice.debug` setter that also sets the logger's level, and/or have a `Chalice(debug=True)` kwarg to make the code linked above behave as expected.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/386</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>['tests/unit/test_app.py', 'chalice/app.py']</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>['Chalice', 'test_can_use_out_of_order_args']</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>[421, 426, 444, 445, 446, 447, 448, 449, 450, 451, 452, 454, 461, 462, 463, 474, 475, 476, 477, 478, 479, 480, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216]</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/ae738bdb4ee0651e5a37ed95b0f5fd111ba5f826...71f153aebfd8ba58b5fc0f1491c99ff55e24c5b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>138</v>
+      </c>
+      <c r="E57" t="n">
+        <v>22</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>@app.schedule No longer supports Rate/Cron object expression</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>A recent commit (afd23d7d729f8383033fe3851bc1de5effd1f22f), added types to the various decorators.  In particular, the `@app.schedule` decorator requires `expression` to be a `str`, which means that it no longer accepts the object type `Rate` or `Cron`.
+I used to be able to do this (and the [Chalice documentation shows this example as well](https://aws.github.io/chalice/topics/events.html#scheduled-events))
+```python
+@app.schedule(Rate(1, unit=Rate.HOURS), name=f"send_call_reminders-{ENV}")
+```
+Now, I have to add a `to_string()` call as follows:
+```python
+@app.schedule(Rate(1, unit=Rate.HOURS).to_string(), name=f"send_call_reminders-{ENV}")
+```
+I'm thinking the type for the `schedule` decorator should probably be `Union[str, ScheduleExpression]`.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/1967</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>['chalice/app.py']</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>['DecoratorAPI']</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>[790, 791]</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/9ee6aac214382d2480c7ea6d5d6b9fdf69f9e870...37266c268e2dbd271e714a74e23a52aaea76dc35</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>138</v>
+      </c>
+      <c r="E58" t="n">
+        <v>22</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Error creating custom domain for websockets</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>When I try to create a custom domain for my websocket the following error occurs:
+```
+Updating custom domain name: api.transferbank.com.br
+Traceback (most recent call last):
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/cli/__init__.py", line 646, in main
+    return cli(obj={})
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/core.py", line 829, in __call__
+    return self.main(*args, **kwargs)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/core.py", line 782, in main
+    rv = self.invoke(ctx)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/core.py", line 1259, in invoke
+    return _process_result(sub_ctx.command.invoke(sub_ctx))
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/core.py", line 1066, in invoke
+    return ctx.invoke(self.callback, **ctx.params)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/core.py", line 610, in invoke
+    return callback(*args, **kwargs)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/click/decorators.py", line 21, in new_func
+    return f(get_current_context(), *args, **kwargs)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/cli/__init__.py", line 206, in deploy
+    deployed_values = d.deploy(config, chalice_stage_name=stage)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/deploy/deployer.py", line 374, in deploy
+    return self._deploy(config, chalice_stage_name)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/deploy/deployer.py", line 390, in _deploy
+    self._executor.execute(plan)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/deploy/executor.py", line 42, in execute
+    getattr(self, '_do_%s' % instruction.__class__.__name__.lower(),
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/deploy/executor.py", line 55, in _do_apicall
+    result = method(**final_kwargs)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/awsclient.py", line 702, in update_domain_name
+    updated_domain_name = self._update_domain_name_v2(kwargs)
+  File "/Users/rafagan/.virtualenvs/tb-websocket-ws/lib/python3.8/site-packages/chalice/awsclient.py", line 802, in _update_domain_name_v2
+    'hosted_zone_id': result_data['HostedZoneId'],
+KeyError: 'HostedZoneId'
+```
+My configuration is:
+```
+"websocket_api_custom_domain": {
+  "domain_name": "api.transferbank.com.br",
+  "certificate_arn": "arn:aws:acm:us-east-1:073289305372:certificate/d995959e-6f7d-4fcb-9c56-bf370ca1a382",
+  "url_prefix": "tb_wst_channel_manager"
+},
+```</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/1531</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>['tests/functional/test_awsclient.py', 'chalice/awsclient.py']</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>['TestUpdateDomainName', 'TestCreateDomainName', 'TypedAWSClient', 'LogEventsResponse = TypedDict(']</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>[66, 67, 68, 69, 70, 71, 72, 73, 74, 474, 505, 517, 519, 522, 524, 527, 529, 530, 531, 532, 533, 534, 535, 536, 540, 553, 554, 558, 700, 759, 779, 781, 784, 786, 789, 791, 792, 793, 794, 795, 796, 797, 798, 802, 817, 821, 859, 888, 1010, 1036, 1037, 1038, 1039, 1040]</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/0902a6cf8f8ba08cdd3c584f9de1099e6bab98a0...1620d07cfd3032faef49b8b2edfaa7d3996c7aaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>138</v>
+      </c>
+      <c r="E59" t="n">
+        <v>22</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Issue using dataclasses.asdict in response body</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi, 
+Btw, I love Chalice. I ran into an issue where I tried to have a body variable in my response as follows:
+```
+@app.route('/private/users', cors=CORS_CONFIG)
+def get_user():
+    user_dicts = [dataclasses.asdict(user) for user in users.list_users()]
+    return Response(
+        status_code=201,
+        headers=CORS_ENABLED_HEADERS,
+        body=user_dicts
+    )
+```
+User is a `@dataclass` file. It's pretty simple: 
+```
+from dataclasses import dataclass
+from typing import List
+from chalicelib.models.Message import Message
+@dataclass(frozen=True)
+class User:
+    user_id: str
+    sms_number: str
+    email_address: str
+    trusted_devices: List[str]
+    conversation_history: List[Message]
+```
+This works when I run `chalice local`. However, when I run `chalice deploy` and try to build, I get this message. 
+```
+  File "/Library/Developer/CommandLineTools/Library/Frameworks/Python3.framework/Versions/3.7/lib/python3.7/symtable.py", line 95, in lookup
+    flags = self._table.symbols[name]
+KeyError: 'user_dicts'
+```
+Full error log here: [chalice_deploy_err.txt](https://github.com/aws/chalice/files/5106624/chalice_deploy_err.txt)
+Replacing the body variable with an empty dict fixes the issue and I can run `chalice deploy`. 
+</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/1494</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>['tests/unit/test_analyzer.py', 'chalice/analyzer.py']</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>['AppViewTransformer', 'SymbolTableTypeInfer', 'test_can_analyze_transfer_manager_methods', 'ChainedSymbolTable', 'get_client_calls_for_app']</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>[73, 74, 75, 271, 272, 275, 276, 277, 278, 279, 501, 502, 705, 706, 707, 708, 709, 710, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751]</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/ff92794973deb396f8b6bf1217a56ff7e90d5df6...b4a8f6d5be8fc08559ff1c1daa2332a297a5fcfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>138</v>
+      </c>
+      <c r="E60" t="n">
+        <v>22</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Unintuitive routes</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I spent a couple of evenings trying to set up a chalice with two routes, always getting the same error:
+```
+botocore.exceptions.ClientError: An error occurred (BadRequestException) when calling the CreateResource operation: Resource's path part must be specified
+```
+After some trial and error, I discovered the following:
+1. The '/' route is a lie
+If you ask for {hostname}/dev/ you will be rudely rejected.
+If you ask for {hostname}/dev it will access route('/')
+1. Trailing / makes chalice cry.
+Originally I had two routes:
+```
+    @app.route('/')
+    @app.route('/login/')
+```
+And got the error above.
+However, if I change the second route to `@app.route('/login')` it works.
+Can anyone explain this?  Or is this really a bug?
+</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/65</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>['tests/unit/test_deployer.py', 'chalice/cli/__init__.py', 'chalice/deployer.py']</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>['deploy', 'Deployer', 'test_multiple_routes_on_single_spine', 'build_url_trie']</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>[134, 135, 136, 137, 118, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 235, 7, 9, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106]</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/fef8f1361f997e54c17df4951798c0016de0c1fd...1da6287aa4562a16b0bc9537662b2715193d1544</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>py</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>aws/chalice</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>138</v>
+      </c>
+      <c r="E61" t="n">
+        <v>22</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>An error occurred (PolicyLengthExceededException) when calling the AddPermission operation</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Policy was not being correctly autogenerated as it did not include DynamoDB permissions, so I added lines manually to .chalice/policy.json, and build using "chalice deploy --no-autogen-policy".
+This has been working just fine for the last day, however when deploying now, I'm getting the following error:
+**botocore.exceptions.ClientError: An error occurred (PolicyLengthExceededException) when calling the AddPermission operation: The final policy size (20789) is bigger than the limit (20480).**
+Nothing has changed in policy.json, and the deploy command was correctly working an hour ago.
+I've tried slimming down .chalice/policy.json, but still getting the same error and the same size report (20789).
+I've tried deleting the Role from AWS and redeploying.  I then get my .chalice/policy.json shown to me and asked if I want to use it, and I select "y".  The same error is presented.
+</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/issues/48</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>['tests/unit/test_deployer.py', 'tests/functional/test_awsclient.py', 'chalice/awsclient.py', 'chalice/deployer.py']</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>['test_cors_adds_required_headers', 'test_can_build_resource_routes_for_single_view', 'TestCanDeleteRolePolicy', 'TypedAWSClient', 'APIGatewayResourceCreator']</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>[182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 268, 269, 275, 276, 277, 278, 279, 280, 281, 282, 287, 303, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 232, 373]</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>https://github.com/aws/chalice/compare/084e2360a9d6f796fa9e7d4de823135908d56267...84fd259a7b84fc697ea181926fe27249ccc714b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>226</v>
+      </c>
+      <c r="E62" t="n">
+        <v>64</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Continuous binary getting swallowed?</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>My WS JS hosted in Chrome seems to be sending the following frames:
+BINARY, isFin = false
+CONTINUOUS, isFin = true
+Java-WebSocket seems to drop the CONTINUOUS frame on the floor and the application never gets it:
+```java
+// org/java_websocket/drafts/Draft_6455.java:542
+} else if( frame.isFin() ) {
+	if( current_continuous_frame == null )
+		throw new InvalidDataException( CloseFrame.PROTOCOL_ERROR, "Continuous frame sequence was not started." );
+	//Check if the whole payload is valid utf8, when the opcode indicates a text
+	if( current_continuous_frame.getOpcode() == Framedata.Opcode.TEXT ) {
+		//Checking a bit more from the frame before this one just to make sure all the code points are correct
+		int off = Math.max( current_continuous_frame.getPayloadData().limit() - 64, 0 );
+		current_continuous_frame.append( frame );
+		if( !Charsetfunctions.isValidUTF8( current_continuous_frame.getPayloadData(), off ) ) {
+			throw new InvalidDataException( CloseFrame.NO_UTF8 );
+		}
+	}
+	// **** What about if the current_continuous_frame.getOpcode() == Framedata.Opcode.BINARY ****//
+	current_continuous_frame = null;
+```
+Is this expected? Is Chrome breaking the spec? Is this something Java-WebSocket should handle differently?</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/564</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/WebSocketListener.java', 'src/main/java/org/java_websocket/WebSocketImpl.java', 'src/main/java/org/java_websocket/drafts/Draft_6455.java', 'src/main/java/org/java_websocket/server/WebSocketServer.java', 'src/test/java/org/java_websocket/example/AutobahnServerTest.java']</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>['class', 'interface', 'abstract']</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>[608, 62, 77, 90, 101, 112, 117, 122, 123, 133, 144, 153, 161, 172, 181, 189, 197, 198, 203, 211, 219, 65, 66, 67, 68, 69, 104, 557, 561, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 580, 591, 592, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 770, 86, 87, 91, 92]</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/f33422e9951369ffd948d473c026ef0e6da6b8e4...32c1ce01c9064d68c8adcfa3b1b577d30bed8cb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>226</v>
+      </c>
+      <c r="E63" t="n">
+        <v>64</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>WebSocketServer freezes in stop() method</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello,
+first I would like to thank you for creating a great and useful library.
+I'am using it in Android application to communicate with website. 
+When I try to stop the server, the application sometimes stops responding.
+The main thread is indefinitely waiting in "WebSocketServer.stop()" method in "selectorThread.join()" line, because the "selectorThread" never ends. This happens because "selectorThread" is waiting in "run()" method in "selector.select()" line.
+Do you know what could be the cause of this behavior?
+Thank you all in advance for any help you can provide.
+Regards,
+Vito
+</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/259</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/server/WebSocketServer.java']</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>['abstract']</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>[219, 220, 221, 222]</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/ac45d846806ad662de48c206896d1248acbb53ff...e4c248a69f0cb36f87e5b3d3100bd2b46e027289</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>226</v>
+      </c>
+      <c r="E64" t="n">
+        <v>64</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Bad rsv 4 on android</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Hello, our team using this library for connecting websocket server on Android platform,
+sometimes,  there are 'bad rsv 4' errors occurred. Seems same problem with #430.
+```
+04-27 14:26:09.960 I/System.out( 1564): D/WebsocketChannel: 000000	48 54 54 50 2f 31 2e 31 20 31 30 31 20 53 77 69 74 63  HTTP/1.1 101 Switc
+04-27 14:26:09.960 D/WebSocketChannel( 1564): onError:org.java_websocket.exceptions.InvalidFrameException: bad rsv 4
+```
+The debug log above shows the **WebSocketImpl** treat the handshake response as normal websocket frame and decode it, then throw an InvalidFrameException.
+Our client tries to reconnect to server endlessly when it is in condition of unstable network environment. 
+So is it possible that method **org.java_websocket.WebSocketImpl#decode**  was invoked after **WebSocketClient** closed in some extreme cases?</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/465</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/WebSocketImpl.java']</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>[154, 155, 156]</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/b983c881b2dfb9f4c607f4b8b8201666e3491a12...2daee16dacbf1e0a9186f260310400a03c10803d</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>226</v>
+      </c>
+      <c r="E65" t="n">
+        <v>64</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Endless loop in client upon close() when using wss</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First, thanks so much for creating the library, it's really useful. I am using this via gottox/socket-io (client) and have run into this nasty problem of an endless loop in SSLSocketChannel2.java when closing a connection (maybe after the other side closed first). A couple of these failures is all it takes to pin the CPU at 100% as the threads that execute these loops pile up.
+I doubt this is the correct fix, but what I did was change the following in SSLSocketChannel2.readRemaining(), which seems to work.
+``` java
+        if( inCrypt.hasRemaining() ) {
+            unwrap();
+            int amount = transfereTo( inData, dst );
+&gt;&gt;&gt;         if (engineStatus == SSLEngineResult.Status.CLOSED) {
+&gt;&gt;&gt;             return -1;
+&gt;&gt;&gt;         }
+            if( amount &gt; 0 )
+                return amount;
+        }
+```
+EDIT by @Davidisudadi: formatted code
+</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/171</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/SSLSocketChannel2.java']</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>[8, 9, 10, 11, 12, 13, 14, 216, 217, 218, 292, 293, 294]</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/05d2e2ed045d955947d944d7111ce3e6758843b6...ea7e061369477bfdf5a0c32bad920c91f8af61fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>226</v>
+      </c>
+      <c r="E66" t="n">
+        <v>64</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Websocket server returning 401; can't handle on client side</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a websocket server that returns 401 on the http handshake
+I can't figure out how to get that information on the websocket client
+Two things I can't figure out:
+1. Where can I get the http status code returned form the server (401 in this case)
+   onClose is called but with irrelevant code (-1) which I saw in your code that it means "never connected"
+2. onError is called but for totally different reason. I get onError ssl == null
+   why would the client library continue to try to decode the handshake, or something like that, when the socket wasn't upgraded (101)? why not just stop there? The ssl error is irrelevant here and is fired do to the fact that the server did not upgrade the socket
+What I did to get the status code from the server was to subclass my own Draft, implement acceptHandshakeAsClient and copyInsance; this gave me access to the handshake response
+When I see that the status code is 401 I return NOT_MATCHED
+This is the only place I saw I can get the status code, but it makes me do ugly things like saving the status code in a variable to be used by onClose and onError which are then called (but with irrelevant data - code == -1 and error exception is ssl == null)
+Thanks
+</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/390</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/WebSocketImpl.java']</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>[450, 451]</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/37b4610cd6c5b5f717b8c4ca196947019a0ed8b1...f1eeff4c3b677a503d04d260475b9725445a82d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>226</v>
+      </c>
+      <c r="E67" t="n">
+        <v>64</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>CONTINUOUS should be decoded depending on the first frame</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**Describe the bug**
+Due to changes with #1165 a return was introduced to handle not decode messages where no RSV1 is set.
+This is however the case for a frame with opcode CONTINUOUS.
+It is a valid framing and should therefore work
+**To Reproduce**
+Steps to reproduce the behavior:
+1. Run autobahn testsuite 
+**Expected behavior**
+autoban testsuite passes
+</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/1230</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/drafts/Draft_6455.java', 'src/main/java/org/java_websocket/extensions/permessage_deflate/PerMessageDeflateExtension.java']</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>[118, 119, 120, 121, 122, 123, 130, 131, 132, 133, 134, 254, 258, 273, 275, 330, 332, 351, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 806, 807, 809, 1142, 1150, 145, 146, 147, 148]</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/2c9b09127fbbc6d73438097a961a1337dd0d8a65...8f1f8e4462b8939f4f1706681d934658c6794bc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>226</v>
+      </c>
+      <c r="E68" t="n">
+        <v>64</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Draft_6455 flagged by Veracode CWE-331 replace Random with SecureRandom</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Our veracode scan flagged usage of `Random` in Draft_6455.java as a vulnerability.
+https://cwe.mitre.org/data/definitions/331.html
+According to Websocket Protocol:
+For example, each masking could be drawn from a cryptographically strong random number generator. If the same key is used or a decipherable pattern exists for how the next key is chosen, the attacker can send a message that, when masked, could appear to be an HTTP request (by taking the message the attacker wishes to see on the wire and masking it with the next masking key to be used, the masking key will effectively unmask the data when the client applies it).
+According to this specification the library should be using SecureRandom to prevent brute force attacks.
+**Environment(please complete the following information):**
+ - Version used: 1.5.1
+ - Java version: 1.8
+ - Operating System and version: Android
+ - Endpoint Name and version:
+ - Link to your project:
+**Additional context**
+Add any other context about the problem here.
+</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/1132</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/drafts/Draft_6455.java']</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>[32, 153]</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/32d5656ffd0aa4ba6caba830ac0205c7bf2609e3...feec867c81d1a426815717b489147894a19826e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>226</v>
+      </c>
+      <c r="E69" t="n">
+        <v>64</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Crash on Android due to missing method `setEndpointIdentificationAlgorithm` on 1.5.0.</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Websocket library 1.5.0
+The same code was not crashing on 1.4.1
+This is the entire stack trace. I got it through Crashlytics so I cannot describe steps that led to it.
+```
+Fatal Exception: java.lang.NoSuchMethodError: No virtual method setEndpointIdentificationAlgorithm(Ljava/lang/String;)V in class Ljavax/net/ssl/SSLParameters; or its super classes (declaration of 'javax.net.ssl.SSLParameters' appears in /system/framework/core-libart.jar)
+       at org.java_websocket.client.WebSocketClient.run(WebSocketClient.java:476)
+       at java.lang.Thread.run(Thread.java:831)
+```
+Android 5.0.1 (API 21).
+Brand: HUAWEI
+Model: P8 Lite
+</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/1011</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>['src/test/java/org/java_websocket/issues/Issue997Test.java', 'src/main/java/org/java_websocket/client/WebSocketClient.java']</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>['class', 'abstract']</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>[521, 526, 527, 528, 146, 147]</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/c207fb8a7c28e7c49bf42e8da7e7866e7db60043...877ad764e5d01166d754e611a4139e816cc04d0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>226</v>
+      </c>
+      <c r="E70" t="n">
+        <v>64</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>IOException wrapped in InternalError not handled properly</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**Describe the bug**
+The call to `socket.connect(...)` at `WebSocketClient:436` can throw a `java.lang.InternalError` that is currently not handled in the enclosing try/catch as it extends `java.lang.Error` and not `java.lang.Exception`
+This `InternalError` wraps a `java.lang.IOException` that contains useful information to the websocket engine to hande this case.
+**To Reproduce**
+Steps to reproduce the behavior:
+1. Install a proxy, i.e. squid
+2. Make it deny connections
+**Example application to reproduce the issue**
+Use the previously installed proxy in the `ProxyClientExample`
+**Expected behavior**
+An IOException handled by the underlying websocket engine
+**Debug log**
+```
+Exception in thread "WebSocketConnectReadThread-11" java.lang.InternalError: Should not reach here
+	at java.net.HttpConnectSocketImpl.doTunneling(HttpConnectSocketImpl.java:181)
+	at java.net.HttpConnectSocketImpl.doTunnel(HttpConnectSocketImpl.java:168)
+	at java.net.HttpConnectSocketImpl.access$200(HttpConnectSocketImpl.java:44)
+	at java.net.HttpConnectSocketImpl$2.run(HttpConnectSocketImpl.java:151)
+	at java.net.HttpConnectSocketImpl$2.run(HttpConnectSocketImpl.java:149)
+	at java.security.AccessController.doPrivileged(Native Method)
+	at java.net.HttpConnectSocketImpl.privilegedDoTunnel(HttpConnectSocketImpl.java:148)
+	at java.net.HttpConnectSocketImpl.connect(HttpConnectSocketImpl.java:111)
+	at java.net.Socket.connect(Socket.java:589)
+	at org.java_websocket.client.WebSocketClient.run(WebSocketClient.java:436)
+	at java.lang.Thread.run(Thread.java:748)
+Caused by: java.lang.reflect.InvocationTargetException
+	at sun.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+	at sun.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:62)
+	at sun.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+	at java.lang.reflect.Method.invoke(Method.java:498)
+	at java.net.HttpConnectSocketImpl.doTunneling(HttpConnectSocketImpl.java:179)
+	... 10 more
+Caused by: java.io.IOException: Unable to tunnel through proxy. Proxy returns "HTTP/1.1 403 Forbidden"
+	at sun.net.www.protocol.http.HttpURLConnection.doTunneling(HttpURLConnection.java:2142)
+	... 15 more
+```
+**Environment(please complete the following information):**
+ - Version used: 1.4.0
+ - Java version: 1.8.0_181
+ - Operating System and version: Ubuntu 16.04 LTS
+ - Endpoint Name and version: "ws://echo.websocket.org"
+ - Link to your project: ProxyClientExample in the examples folder
+**Additional context**
+This is my first time reporting an issue on a open source project.
+I'm open to feedback :)
+</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/905</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/client/WebSocketClient.java']</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>['abstract']</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>[31, 484, 485, 486, 487, 488, 489, 490, 491, 492]</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/c9e75337940cd041e935191e3dbec0005a622c64...f73cca0f3faf1bc5d72ba44d0ee42a1b6dabe28e</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>226</v>
+      </c>
+      <c r="E71" t="n">
+        <v>64</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Exclude default port from wss host</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>&lt;!--- Provide a general summary of the issue in the Title above --&gt;
+I'm working with a server balanced by a proxy that redirect my request to the targeted server depends on the URL I requested.
+One of these servers has a secure Websocket (I mean wss) and it works on the default port (443).
+In your client (class WebSocketClient.java) you avoid to include the port in the host by: `port != WebSocket.DEFAULT_PORT ? ":" + port : ""`, but this works only for ws default port and not for wss that now is including ":443" at the end of the host. In my app, for example I want to connect to "wss://app.example.com" and without this check it's trying to connect to "wss://app.example.com:443" and the proxy cannot resolve this host.
+## Possible Solution
+Adding a check for DEFAULT_WSS_PORT as well as the check for DEFAULT_PORT it solves the problem.
+```java
+String host = uri.getHost() + ( 
+			(port != WebSocket.DEFAULT_PORT &amp;&amp; port != WbSocket.DEFAULT_WSS_PORT)
+			? ":" + port : "" );
+```</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>https://github.com/TooTallNate/Java-WebSocket/issues/685</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>['src/main/java/org/java_websocket/client/WebSocketClient.java']</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>['abstract']</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>[437, 438, 439, 440]</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>https://github.com/tootallnate/java-websocket/compare/c08be4e43f2414d34ecd5b2fa9985f9e4ff48263...8a9df49a0e9fb7bedc0a08e10bed0862a28b9440</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>166</v>
+      </c>
+      <c r="E72" t="n">
+        <v>78</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Stabilizer not Failing,  error go unreported</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Due to a simple error in test code I found this in worker.log
+```
+grepall worker.log iCacheCas
+./worker-10.184.184.149-1-server/worker.log
+INFO  2014-09-11 12:48:24,900 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Initializing test iCacheCas ---------------------------
+      id=iCacheCas
+INFO  2014-09-11 12:48:26,081 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.setup() ------------------------------------
+FATAL 2014-09-11 12:48:26,081 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.setup() ---------------------------
+INFO  2014-09-11 12:48:28,098 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localWarmup() ------------------------------------
+INFO  2014-09-11 12:48:28,098 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localWarmup() ---------------------------
+INFO  2014-09-11 12:48:32,115 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Skipping iCacheCas.run(); member is passive ------------------------------------
+INFO  2014-09-11 12:50:33,277 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- iCacheCas.stop() ------------------------------------
+INFO  2014-09-11 12:50:36,310 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localVerify() ------------------------------------
+INFO  2014-09-11 12:50:36,310 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localVerify() ---------------------------
+INFO  2014-09-11 12:50:41,327 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localTeardown() ------------------------------------
+FATAL 2014-09-11 12:50:41,327 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.localTeardown() ---------------------------
+./worker-10.67.172.55-2-client/worker.log
+INFO  2014-09-11 12:48:25,439 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Initializing test iCacheCas ---------------------------
+      id=iCacheCas
+INFO  2014-09-11 12:48:26,623 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.setup() ------------------------------------
+FATAL 2014-09-11 12:48:26,715 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.setup() ---------------------------
+INFO  2014-09-11 12:48:28,701 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localWarmup() ------------------------------------
+INFO  2014-09-11 12:48:28,702 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localWarmup() ---------------------------
+INFO  2014-09-11 12:48:32,717 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.run() ------------------------------------
+FATAL 2014-09-11 12:48:32,717 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed to execute iCacheCas.run() ------------------------------------
+INFO  2014-09-11 12:50:33,875 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- iCacheCas.stop() ------------------------------------
+INFO  2014-09-11 12:50:36,889 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localVerify() ------------------------------------
+INFO  2014-09-11 12:50:36,889 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localVerify() ---------------------------
+INFO  2014-09-11 12:50:41,916 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localTeardown() ------------------------------------
+FATAL 2014-09-11 12:50:41,916 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.localTeardown() ---------------------------
+./worker-10.184.184.149-2-client/worker.log
+INFO  2014-09-11 12:48:25,409 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Initializing test iCacheCas ---------------------------
+      id=iCacheCas
+INFO  2014-09-11 12:48:26,578 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.setup() ------------------------------------
+FATAL 2014-09-11 12:48:26,689 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.setup() ---------------------------
+INFO  2014-09-11 12:48:28,590 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localWarmup() ------------------------------------
+INFO  2014-09-11 12:48:28,590 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localWarmup() ---------------------------
+INFO  2014-09-11 12:48:32,608 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.run() ------------------------------------
+FATAL 2014-09-11 12:48:32,609 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed to execute iCacheCas.run() ------------------------------------
+INFO  2014-09-11 12:50:33,769 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- iCacheCas.stop() ------------------------------------
+INFO  2014-09-11 12:50:36,795 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localVerify() ------------------------------------
+INFO  2014-09-11 12:50:36,795 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localVerify() ---------------------------
+INFO  2014-09-11 12:50:41,821 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localTeardown() ------------------------------------
+FATAL 2014-09-11 12:50:41,821 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.localTeardown() ---------------------------
+./worker-10.67.172.55-1-server/worker.log
+INFO  2014-09-11 12:48:25,857 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Initializing test iCacheCas ---------------------------
+      id=iCacheCas
+INFO  2014-09-11 12:48:27,000 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.setup() ------------------------------------
+FATAL 2014-09-11 12:48:27,000 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.setup() ---------------------------
+INFO  2014-09-11 12:48:29,020 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localWarmup() ------------------------------------
+INFO  2014-09-11 12:48:29,020 [Thread-3] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localWarmup() ---------------------------
+INFO  2014-09-11 12:48:31,028 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.globalWarmup() ------------------------------------
+FATAL 2014-09-11 12:48:31,044 [Thread-4] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.globalWarmup() ---------------------------
+INFO  2014-09-11 12:48:33,037 [Thread-5] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Skipping iCacheCas.run(); member is passive ------------------------------------
+INFO  2014-09-11 12:50:33,199 [Thread-0] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- iCacheCas.stop() ------------------------------------
+INFO  2014-09-11 12:50:35,213 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.globalVerify() ------------------------------------
+FATAL 2014-09-11 12:50:35,213 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.globalVerify() ---------------------------
+INFO  2014-09-11 12:50:37,223 [Thread-7] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localVerify() ------------------------------------
+INFO  2014-09-11 12:50:37,224 [Thread-7] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.localVerify() ---------------------------
+INFO  2014-09-11 12:50:39,235 [Thread-8] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.globalTeardown() ------------------------------------
+INFO  2014-09-11 12:50:39,235 [Thread-8] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Finished iCacheCas.globalTeardown() ---------------------------
+INFO  2014-09-11 12:50:42,266 [Thread-9] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Starting iCacheCas.localTeardown() ------------------------------------
+FATAL 2014-09-11 12:50:42,266 [Thread-9] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.localTeardown() ---------------------------
+```
+While Stabilizer reported 
+```
+INFO  12:48:24 iCacheCas iCacheCas Starting Test initialization
+INFO  12:48:25 iCacheCas Completed Test initialization
+INFO  12:48:25 iCacheCas Starting Test setup
+INFO  12:48:27 iCacheCas Completed Test setup
+INFO  12:48:28 iCacheCas Starting Test local warmup
+INFO  12:48:30 iCacheCas Completed Test local warmup
+INFO  12:48:30 iCacheCas Starting Test global warmup
+INFO  12:48:32 iCacheCas Completed Test global warmup
+INFO  12:48:32 iCacheCas Starting Test start
+INFO  12:48:33 iCacheCas Completed Test start
+INFO  12:48:33 iCacheCas Test will run for 00d 00h 02m 00s
+INFO  12:49:03 iCacheCas Running 00d 00h 00m 30s, 25.00 percent complete
+INFO  12:49:33 iCacheCas Running 00d 00h 01m 00s, 50.00 percent complete
+INFO  12:50:03 iCacheCas Running 00d 00h 01m 30s, 75.00 percent complete
+INFO  12:50:33 iCacheCas Running 00d 00h 02m 00s, 100.00 percent complete
+INFO  12:50:33 iCacheCas Test finished running
+INFO  12:50:33 iCacheCas Starting Test stop
+INFO  12:50:34 iCacheCas Completed Test stop
+INFO  12:50:34 iCacheCas Starting Test global verify
+INFO  12:50:36 iCacheCas Completed Test global verify
+INFO  12:50:36 iCacheCas Starting Test local verify
+INFO  12:50:38 iCacheCas Completed Test local verify
+INFO  12:50:38 iCacheCas Starting Test global tear down
+INFO  12:50:40 iCacheCas Finished Test global tear down
+INFO  12:50:40 iCacheCas Starting Test local tear down
+INFO  12:50:42 iCacheCas Completed Test local tear down
+INFO  12:50:42 Terminating workers
+INFO  12:50:42 All workers have been terminated
+INFO  12:50:42 Starting cool down (10 sec)
+INFO  12:50:52 Finished cool down
+INFO  12:50:52 Total running time: 147 seconds
+INFO  12:50:52 -----------------------------------------------------------------------------
+INFO  12:50:52 No failures have been detected!
+INFO  12:50:52 -----------------------------------------------------------------------------
+```
+details of setup error
+```
+due to a simple error in my test setup method,  I found this error in worker.log
+```
+FATAL 2014-09-11 12:48:26,081 [Thread-2] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.setup() ---------------------------
+FATAL 2014-09-11 12:48:26,082 [Thread-2] com.hazelcast.stabilizer.tests.utils.ExceptionReporter: Exception detected
+java.lang.NullPointerException: Retrieving a list instance with a null name is not allowed!
+    at com.hazelcast.instance.HazelcastInstanceImpl.getList(HazelcastInstanceImpl.java:208)
+    at com.hazelcast.instance.HazelcastInstanceProxy.getList(HazelcastInstanceProxy.java:91)
+    at com.hazelcast.stabilizer.tests.icache.CasICacheTest.setup(CasICacheTest.java:66)
+    at sun.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+    at sun.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:57)
+    at sun.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+    at java.lang.reflect.Method.invoke(Method.java:606)
+    at com.hazelcast.stabilizer.worker.TestContainer.invoke(TestContainer.java:138)
+    at com.hazelcast.stabilizer.worker.TestContainer.setup(TestContainer.java:101)
+    at sun.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+    at sun.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:57)
+    at sun.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+    at java.lang.reflect.Method.invoke(Method.java:606)
+    at com.hazelcast.stabilizer.worker.MemberWorker$TestCommandRequestProcessingThread$2.doRun(MemberWorker.java:405)
+    at com.hazelcast.stabilizer.worker.MemberWorker$CommandThread.run(MemberWorker.java:493)
+```
+And due to a simple error in localTeardown
+```
+FATAL 2014-09-11 12:50:41,327 [Thread-6] com.hazelcast.stabilizer.worker.MemberWorker: --------------------------- Failed iCacheCas.localTeardown() ---------------------------
+FATAL 2014-09-11 12:50:41,327 [Thread-6] com.hazelcast.stabilizer.tests.utils.ExceptionReporter: Exception detected
+java.lang.NullPointerException
+    at com.hazelcast.stabilizer.tests.icache.CasICacheTest.teardown(CasICacheTest.java:82)
+    at sun.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+    at sun.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:57)
+    at sun.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+    at java.lang.reflect.Method.invoke(Method.java:606)
+    at com.hazelcast.stabilizer.worker.TestContainer.invoke(TestContainer.java:138)
+    at com.hazelcast.stabilizer.worker.TestContainer.localTeardown(TestContainer.java:109)
+    at sun.reflect.NativeMethodAccessorImpl.invoke0(Native Method)
+    at sun.reflect.NativeMethodAccessorImpl.invoke(NativeMethodAccessorImpl.java:57)
+    at sun.reflect.DelegatingMethodAccessorImpl.invoke(DelegatingMethodAccessorImpl.java:43)
+    at java.lang.reflect.Method.invoke(Method.java:606)
+    at com.hazelcast.stabilizer.worker.MemberWorker$TestCommandRequestProcessingThread$2.doRun(MemberWorker.java:405)
+    at com.hazelcast.stabilizer.worker.MemberWorker$CommandThread.run(MemberWorker.java:493)
+```
+```
+</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/292</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>['stabilizer/src/main/java/com/hazelcast/stabilizer/tests/utils/ExceptionReporter.java', 'stabilizer/src/main/java/com/hazelcast/stabilizer/worker/MemberWorker.java']</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>[18, 34, 35, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 53, 54, 349, 368, 372, 376, 377, 399, 419, 420, 497]</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/102611f184ba8e097e82e8695398e3afcf551f57...789659dfe2e6bdf65e9ac98a4351511e7b083852</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>166</v>
+      </c>
+      <c r="E73" t="n">
+        <v>78</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>SIMULATOR_USER rename warning</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>If the old 'USER' is found in Simulator properties, a big fat error should be given</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/1324</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>['simulator/src/test/java/com/hazelcast/simulator/common/SimulatorPropertiesTest.java', 'simulator/src/main/java/com/hazelcast/simulator/common/SimulatorProperties.java']</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>[122, 130, 131, 132, 133, 9, 242, 243, 244, 245, 246, 247, 248, 249]</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/4c9b5b845a6d75f002b25e6127bf986ff4f8fc71...6e7f9dc259f0925cef9a99c36f09e2dc95df08d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>166</v>
+      </c>
+      <c r="E74" t="n">
+        <v>78</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Problem starting members, doesn't lead to failure</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When there is a problem starting members, this isn't translated to a nice and useful message
+```
+INFO  11:25:49 =========================================================================
+INFO  11:25:49 Starting 2 Workers (2 members, 0 clients)...
+FATAL 11:25:50 Could not create 1 member Worker on C_A1 (EXCEPTION_DURING_OPERATION_EXECUTION)
+FATAL 11:25:50 [C_A2] Failed to start Worker: Failed to start Worker
+FATAL 11:25:51 [C_A1] Failed to start Worker: Failed to start Worker
+INFO  11:25:51 Terminating 0 Workers...
+INFO  11:25:52 Waiting up to 120 seconds for shutdown of 0 Workers...
+INFO  11:25:52 Finished shutdown of all Workers (0 seconds)
+INFO  11:25:52 Shutdown of com.hazelcast.simulator.protocol.connector.CoordinatorConnector...
+INFO  11:25:52 ServerConnectorMessageQueueThread received POISON_PILL and will stop...
+INFO  11:25:52 HarakiriMonitor is enabled and will kill inactive EC2 instances after 7200 seconds
+INFO  11:25:52 Stopping 2 Agents...
+INFO  11:25:52 Stopping Agent 54.158.82.62
+INFO  11:25:52 Stopping Agent 54.205.232.99
+INFO  11:25:54 Starting HarakiriMonitor on 54.205.232.99
+INFO  11:25:54 Starting HarakiriMonitor on 54.158.82.62
+INFO  11:25:56 Successfully stopped 2 Agents
+INFO  11:25:56 Download artifacts of 2 machines...
+INFO  11:25:56 Downloading Worker logs from 54.205.232.99
+INFO  11:25:56 Downloading Worker logs from 54.158.82.62
+INFO  11:25:56 Downloading Agent logs from 54.158.82.62
+INFO  11:25:56 Downloading Agent logs from 54.205.232.99
+INFO  11:26:04 Finished downloading artifacts of 2 machines (7 seconds)
+INFO  11:26:04 Executing after-completion script: /home/alarmnummer/hazelcast-simulator-0.9-RC1-SNAPSHOT/conf/after-completion.sh
+INFO  11:26:04 Finished after-completion script
+INFO  11:26:04 =========================================================================
+INFO  11:26:04 No failures have been detected!
+INFO  11:26:04 =========================================================================
+```
+</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/1248</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/common/FailureType.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/FailureCollector.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/operation/FailureOperation.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/CoordinatorRunMonolith.java']</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>['class', 'enum', 'CoordinatorRunMonolith']</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>[30, 31, 19, 21, 53, 54, 55, 56, 57, 58, 59, 18, 66, 67, 68, 69, 70, 71, 73, 74, 75, 76, 77, 78, 80, 81, 82, 83, 114, 115, 116, 117, 45, 52]</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/c7af9b0b66fb0f19692b00e9c4d1d79c4f2ba165...5c913ce771a28a5d33056be57e5fbae3649aee77</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>166</v>
+      </c>
+      <c r="E75" t="n">
+        <v>78</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Bug in harakiri</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>The problem is in the startup of the harakiri monitor after a test completes. Instead of setting the actual key/value, the literal values are taken. So if you have your identity configured as '''bla/ec2.identity''', then '''bla/ec2.identity''' is the literal value.
+The cause of this is the SimulatorProperties.asMap function which returns the values without replacements being applied.</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/1423</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/common/SimulatorProperties.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/AgentUtils.java', 'simulator/src/main/java/com/hazelcast/simulator/utils/CloudProviderUtils.java']</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>['class', 'final']</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>[29, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 31, 33, 50, 51, 52, 53, 54, 55]</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/d8d4ebf4f4b0b67e99d1cf289868b0daa41dee83...db6a948f879dfacba235f8a67774256782100bb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>166</v>
+      </c>
+      <c r="E76" t="n">
+        <v>78</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Parallel test suites</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Currently test suites can't be run in parallel, because in the Agent only 1 testsuite can be active.
+</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/1130</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/protocol/processors/AgentOperationProcessor.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/FailureHandlerImpl.java', 'simulator/src/test/java/com/hazelcast/simulator/coordinator/FailureCollectorTest.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/operation/OperationType.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/registry/TestData.java', 'simulator/src/test/java/com/hazelcast/simulator/protocol/processors/CoordinatorOperationProcessorTest.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/FailureCollector.java', 'simulator/src/test/java/com/hazelcast/simulator/coordinator/RunTestSuiteTaskTest.java', 'simulator/src/test/java/com/hazelcast/simulator/protocol/processors/AgentOperationProcessorTest.java', 'simulator/src/test/java/com/hazelcast/simulator/protocol/ProtocolUtil.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/Agent.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/Coordinator.java', 'simulator/src/test/java/com/hazelcast/simulator/agent/FailureHandlerImplTest.java', 'simulator/src/test/java/com/hazelcast/simulator/agent/AgentSmokeTest.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/operation/FailureOperation.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/RunTestSuiteTask.java', 'simulator/src/test/java/com/hazelcast/simulator/protocol/operation/FailureOperationTest.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/registry/ComponentRegistry.java', 'simulator/src/test/java/com/hazelcast/simulator/protocol/registry/ComponentRegistryTest.java', 'simulator/src/main/java/com/hazelcast/simulator/protocol/operation/InitTestSuiteOperation.java']</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>['class', 'FailureHandlerImpl', 'final', 'enum', 'ProtocolUtil']</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>[45, 87, 69, 101, 20, 21, 52, 54, 56, 68, 69, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 69, 71, 74, 79, 88, 40, 45, 49, 60, 61, 62, 63, 64, 50, 51, 52, 53, 54, 32, 247, 271, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 286, 289, 290, 291, 292, 293, 294, 295, 296, 19, 27, 29, 33, 47, 48, 49, 50, 103, 225, 6, 30, 35, 36, 42, 45, 48, 8, 34, 66, 95, 96, 102, 199, 213, 314, 442, 22, 167, 168, 38, 17, 58, 67, 69, 11, 20, 285, 287, 293, 294, 295, 296, 297, 298, 299, 300, 301, 303, 305, 306, 307, 308]</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/9b79fa3cfdefab472e5e1c0261150e7e8a51d75d...2d5d77202337d6bc369d1f45f5a4fc91d3447f24</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>166</v>
+      </c>
+      <c r="E77" t="n">
+        <v>78</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Remote: when fail fast, test not aborting</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When deliberately causing a test failure by killing the members (and having the load generated by a client),the testcase runner doesn't complete
+```
+INFO  14:49:10 AtomicLongTest Running 00d 00h 00m 20s (  6.67%)        54,600 ops     3,409.70 ops/s        292 µs (avg)      2,619 µs (99.9th)     19,628 µs (max)
+INFO  14:49:15 Valid connection from /127.0.0.1:39036 (magic bytes found)
+INFO  14:49:15 Killing working....
+INFO  14:49:15 Kill send to worker [C_A2_W1]
+INFO  14:49:20 AtomicLongTest Running 00d 00h 00m 30s ( 10.00%)        92,414 ops     3,781.40 ops/s        263 µs (avg)      1,140 µs (99.9th)     21,725 µs (max)
+INFO  14:49:30 AtomicLongTest Running 00d 00h 00m 40s ( 13.33%)        92,915 ops        50.10 ops/s        295 µs (avg)      2,059 µs (99.9th)      2,772 µs (max)
+INFO  14:49:40 AtomicLongTest Running 00d 00h 00m 50s ( 16.67%)       153,606 ops     6,069.10 ops/s        326 µs (avg)        332 µs (99.9th) 10,015,997 µs (max)
+INFO  14:49:41 Valid connection from /127.0.0.1:39208 (magic bytes found)
+INFO  14:49:41 Killing working....
+INFO  14:49:41 Kill send to worker [C_A1_W1]
+ERROR 14:49:47 Failure #1 C_A1_W3 run-AtomicLongTest WORKER_EXCEPTION[com.hazelcast.spi.exception.TargetDisconnectedException: Disconnecting from member [10.30.221.14]:5701 due to heartbeat problems. Current time: 2016-08-23 07:49:47.151. Last heartbeat requested: 2016-08-23 07:49:30.151. Last heartbeat received: 2016-08-23 07:49:30.153. Last read: 2016-08-23 07:49:46.307. Connection ClientConnection{live=false, connectionId=2, socketChannel=DefaultSocketChannelWrapper{socketChannel=java.nio.channels.SocketChannel[closed]}, remoteEndpoint=[10.30.221.14]:5701, lastReadTime=2016-08-23 07:49:46.307, lastWriteTime=2016-08-23 07:49:46.305, closedTime=2016-08-23 07:49:46.307, lastHeartbeatRequested=2016-08-23 07:49:30.151, lastHeartbeatReceived=2016-08-23 07:49:30.153}]
+INFO  14:49:50 AtomicLongTest Running 00d 00h 01m 00s ( 20.00%)       195,126 ops     4,151.58 ops/s        145 µs (avg)        256 µs (99.9th)     27,918 µs (max)
+INFO  14:49:50 AtomicLongTest Critical failure detected, aborting run phase
+INFO  14:49:51 AtomicLongTest Test finished running
+INFO  14:49:51 AtomicLongTest Executing Test stop
+ERROR 14:52:51 Failure #2 C_A1_W3 WORKER_TIMEOUT[Worker has not sent a message for 180 seconds]
+```
+I guess it is waiting for the old member count, not the current member count.
+</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/1123</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/agent/FailureSender.java', 'simulator/src/test/java/com/hazelcast/simulator/agent/workerprocess/WorkerProcessFailureMonitorTest.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/FailureSenderImpl.java', 'simulator/src/test/java/com/hazelcast/simulator/agent/FailureSenderImplTest.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/workerprocess/WorkerProcessManager.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/Agent.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/workerprocess/WorkerProcessFailureMonitor.java', 'simulator/src/main/java/com/hazelcast/simulator/coordinator/Coordinator.java', 'simulator/src/main/java/com/hazelcast/simulator/agent/workerprocess/WorkerProcess.java']</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>['class', 'final', 'FailureSenderImpl']</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>[58, 77, 18, 34, 36, 45, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 74, 85, 91, 98, 101, 16, 20, 22, 36, 99, 100, 101, 102, 103, 104, 105, 106, 35, 46, 49, 52, 56, 85, 93, 100, 163, 201, 231, 47, 48, 49, 50, 431, 433, 435, 437, 34, 37, 45, 67, 73, 81, 93, 104, 59, 72, 73, 80, 96, 100, 107, 125, 134, 142, 147, 156, 170, 183, 196, 202, 214, 221, 231, 244, 255, 267, 274, 288, 299, 315, 327, 337, 397, 398, 401, 402, 405, 406, 411]</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/86e080b937212589215b80309a3bef116e9da3f9...c3e7b452eb6aa26fe305dd41ab7ed91641aa9da7</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>166</v>
+      </c>
+      <c r="E78" t="n">
+        <v>78</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Race in PerformanceStateContainer</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Because queue's are swapped, it can happen that a performancestate is added to a queue that moments later gets swapped out and processed. So you get an unprocessed PerformanceState on the queue which will never been seen
+</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/854</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/coordinator/PerformanceStateContainer.java']</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>[64, 65, 66, 69, 80, 81, 82, 117, 118, 124, 125, 126, 127, 128, 129, 130, 131, 133, 135]</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/752e35a5e13d13210e8b2793dd0be0e18a5bf9cf...74e25d4fc23495e8ddf8ac5729e48a1e6976413e</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>166</v>
+      </c>
+      <c r="E79" t="n">
+        <v>78</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>InterruptedException in PerformanceThread.run()</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happens from time to time when using external clients (don't know if it will fail on regular tests as well). It's after the testsuite completes, so performance results and probes are written. Maybe it's just not shutdown properly.
+```
+FATAL 13:58:43 Exception in PerformanceThread.run()
+java.lang.RuntimeException: java.lang.InterruptedException
+    at com.hazelcast.simulator.coordinator.remoting.AgentsClient.getAllFutures(AgentsClient.java:394)
+    at com.hazelcast.simulator.coordinator.remoting.AgentsClient.executeOnAllWorkersDetailed(AgentsClient.java:333)
+    at com.hazelcast.simulator.coordinator.PerformanceMonitor$PerformanceThread.checkPerformance(PerformanceMonitor.java:110)
+    at com.hazelcast.simulator.coordinator.PerformanceMonitor$PerformanceThread.run(PerformanceMonitor.java:99)
+Caused by: java.lang.InterruptedException
+    at java.util.concurrent.FutureTask.awaitDone(FutureTask.java:404)
+    at java.util.concurrent.FutureTask.get(FutureTask.java:204)
+    at com.hazelcast.simulator.coordinator.remoting.AgentsClient.getAllFutures(AgentsClient.java:381)
+    ... 3 more
+```
+</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/699</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/coordinator/remoting/AgentsClient.java']</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>[14, 395, 396, 397]</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/76278f9af558824f99db2bbed90e23f072a48d2c...9aedd37210ec8519c8821ff4666c20453128cf0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>166</v>
+      </c>
+      <c r="E80" t="n">
+        <v>78</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>IllegalThreadStateException for WorkerPerformanceMonitorThread</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">```
+Failure[
+   message='Worked ran into an unhandled exception'
+   type='Worker exception'
+   agentAddress=10.184.183.169
+   time=Tue May 19 15:52:34 UTC 2015
+   workerAddress=10.184.183.169:5702
+   workerId=worker-10.184.183.169-1-server
+   test=null unknown
+   cause=java.lang.IllegalThreadStateException
+        at java.lang.Thread.start(Thread.java:705)
+        at com.hazelcast.simulator.worker.WorkerPerformanceMonitor.start(WorkerPerformanceMonitor.java:36)
+        at com.hazelcast.simulator.worker.WorkerCommandRequestProcessor$WorkerCommandRequestProcessorThread.process(WorkerCommandRequestProcessor.java:195)
+        at com.hazelcast.simulator.worker.WorkerCommandRequestProcessor$WorkerCommandRequestProcessorThread.doProcess(WorkerCommandRequestProcessor.java:121)
+        at com.hazelcast.simulator.worker.WorkerCommandRequestProcessor$WorkerCommandRequestProcessorThread.run(WorkerCommandRequestProcessor.java:106)
+]
+```
+why for this super complex start?
+```
+ boolean start() {
+        if (!thread.running) {
+            synchronized (this) {
+                if (!thread.running) {
+                    thread.running = true;
+                    thread.start();
+                    return true;
+                }
+            }
+        }
+        return false;
+    }
+```
+</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/643</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/worker/WorkerPerformanceMonitor.java']</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>['WorkerPerformanceMonitor']</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>[13, 26, 27, 30, 34, 35, 37, 38, 39, 43, 46, 48, 58, 60, 71]</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/7e4e7522e008a12fb2374ba28389b719500b4dfa...80dbe23bb577efeca7e6cb999f50a39022be532e</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>166</v>
+      </c>
+      <c r="E81" t="n">
+        <v>78</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>NPE in Provisioner when Simulator was compiled without git metadata</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you e.g. download the Simulator sources as ZIP archive from GitHub there is no git repository/metadata available.
+If you compile Simulator and use it, the `Provisioner` fails with a NPE, because it tries to print the git revision of Simulator, which is not available in that case.
+The issue will be the underlaying `GitInfo` which should not fail in that case.
+```
+INFO  16:27:13 Hazelcast Simulator Provisioner
+Exception in thread "main" java.lang.ExceptionInInitializerError
+    at com.hazelcast.simulator.provisioner.Provisioner.main(Provisioner.java:457)
+Caused by: java.lang.NullPointerException
+    at java.util.Properties$LineReader.readLine(Properties.java:434)
+    at java.util.Properties.load0(Properties.java:353)
+    at java.util.Properties.load(Properties.java:341)
+    at com.hazelcast.simulator.common.GitInfo.loadGitProperties(GitInfo.java:56)
+    at com.hazelcast.simulator.common.GitInfo.&lt;init&gt;(GitInfo.java:28)
+    at com.hazelcast.simulator.common.GitInfo.&lt;clinit&gt;(GitInfo.java:23)
+    ... 1 more
+```
+</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/issues/629</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>['simulator/src/main/java/com/hazelcast/simulator/common/GitInfo.java', 'simulator/src/test/java/com/hazelcast/simulator/common/GitInfoTest.java']</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>['class', 'final']</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>[13, 14, 15, 16, 17, 18, 19, 20, 21, 30, 53, 56, 57, 58, 59, 60, 62, 64, 65, 71, 72, 5, 6, 7, 8, 10, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65]</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>https://github.com/hazelcast/hazelcast-simulator/compare/2cd2b5f6ec58a86e6287b392c74fa48435067f3e...6dde8d581d726021da748f499628911e2905abf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>173</v>
+      </c>
+      <c r="E82" t="n">
+        <v>104</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Uninformative error message in CLI when missing spaces before 'required' keyword</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When there are missing spaces before input's 'required' keyword, for example:
+flow:
+  inputs:
+    - input:
+      required: true
+ and trying to run the flow in the CLI, you get an uninformative error message:
+Command failed java.lang.RuntimeException: java.lang.RuntimeException: Error transforming source: flow_with_required_input.sl to a Slang model. null
+</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/199</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>['cloudslang-compiler/src/main/java/io/cloudslang/lang/compiler/modeller/transformers/AbstractInputsTransformer.java']</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>['abstract']</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>[37]</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/847c906f25e97c48a9058c653eca079659fe3e42...d232e7828e7a803967f05215517891c75e2f0797</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>173</v>
+      </c>
+      <c r="E83" t="n">
+        <v>104</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>False validation error</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">if an input has the tag private: true, it should not be accessible to the user at runtime:
+&gt; 11:36:02 [ERROR] Failed to extract metadata for file: 'c:\\Users\\moldovas\\cloudslang\\cloud-slang-content\\content\\io\\cloudslang\\base\\datetime\\get_time.sl'.
+&gt; Error for executable io.cloudslang.base.datetime.get_time: Input 'localeLang' is missing description.
+&gt; 
+&gt; ```
+&gt; - localeLang:
+&gt;     default: ${get("locale_lang", "en")}
+&gt;     private: true
+&gt; ```
+</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/868</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>['cloudslang-content-verifier/src/test/java/io/cloudslang/lang/tools/build/validation/StaticValidatorTest.java', 'cloudslang-content-verifier/src/main/java/io/cloudslang/lang/tools/build/validation/StaticValidatorImpl.java']</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>[16, 59, 60, 57, 58, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85]</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/70d43050c2f180b18170be7135e85e939f8405ce...5b1aadbf21f9837d2cd7edaf0fa445af6149d41e</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>173</v>
+      </c>
+      <c r="E84" t="n">
+        <v>104</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>CLI compile folders</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>`compile dir_with_no_sl_files` --&gt; NPE
+compile description says `--f ...` &lt;-- should be updated to `--d`</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/956</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>['cloudslang-cli/src/main/java/io/cloudslang/lang/cli/services/ConsolePrinterImpl.java', 'cloudslang-cli/src/test/java/io/cloudslang/lang/cli/services/ConsolePrinterImplTest.java', 'cloudslang-cli/src/main/java/io/cloudslang/lang/cli/SlangCli.java']</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>[38, 39, 40, 41, 42, 43, 44, 45, 46, 151, 152, 154, 155, 172, 173, 174, 175, 176, 177, 178, 179, 180, 186, 196, 222, 51, 52, 53, 45, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114]</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/542fca98f64398385726a81f29ce55419d206129...d611268b66a76eb27258717238591ed7529f497a</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>173</v>
+      </c>
+      <c r="E85" t="n">
+        <v>104</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>CLI log: Missing CALL_ARGUMENTS for Python action [1]</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Observed the following in CLI log:
+Java action - call arguments logged:
+```
+STEP_TYPE=ACTION, STEP_NAME=null, TYPE=EVENT_ACTION_START, CALL_ARGUMENTS={characterSet=UTF-8, agentForwarding=null, command=docker ps -a, timeout=600000, password=null, pty=false, privateKeyFile=c:/.../id_rsa, port=22, host=111.111.111.111, arguments=null, closeSession=false, username=core}
+```
+Python action - call arguments not logged:
+```
+STEP_TYPE=ACTION, STEP_NAME=null, TYPE=EVENT_ACTION_START, CALL_ARGUMENTS={}
+```
+however there are inputs declared in the operation.
+Shouldn't call arguments appear in the log also for Python actions (EVENT_ACTION_START events)?
+</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/331</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>['cloudslang-runtime/src/main/java/io/cloudslang/lang/runtime/events/LanguageEventData.java', 'cloudslang-runtime/src/main/java/io/cloudslang/lang/runtime/steps/ActionSteps.java', 'cloudslang-runtime/src/test/java/io/cloudslang/lang/runtime/steps/ActionStepsTest.java']</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>[155, 156, 157, 158, 159, 20, 21, 23, 34, 63, 64, 65, 66, 67, 68, 72, 18, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200]</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/b57a401b31e480701af163aec446c0dfb0c6ede2...c1ec95f59f4c904eed6bd03915a553d1bfbac616</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>173</v>
+      </c>
+      <c r="E86" t="n">
+        <v>104</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Builder - file name not printed</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://travis-ci.org/CloudSlang/cloud-slang-content/builds/238929220?utm_source=github_status&amp;utm_medium=notification
+```console
+02/06/17 22:05:30 [INFO] Test case passed: testRemoteSecureCopySucessLocalToRemote [/home/travis/build/CloudSlang/cloud-slang-content/test/io/cloudslang/base/remote_file_transfer/remote_secure_copy.inputs.yaml]. Finished running: io.cloudslang.base.remote_file_transfer.test_remote_secure_copy_local_to_remote with result: SUCCESS
+02/06/17 22:05:30 [ERROR]
+02/06/17 22:05:30 [ERROR] ------------------------------------------------------------
+02/06/17 22:05:30 [ERROR] Exception: Error at line [13] - There should be an empty line between two sections of different tags (@description and @input)
+02/06/17 22:05:30 [ERROR] Exception: Error at line [13] - There should be an empty line between two sections of different tags (@description and @input)
+02/06/17 22:05:30 [ERROR] Exception: Error at line [11] - There should be an empty line between two sections of different tags (@description and @input)
+02/06/17 22:05:30 [ERROR] Exception: Error at line [12] - There should be an empty line between two sections of different tags (@description and @input)
+02/06/17 22:05:30 [ERROR] FAILURE: Validation of slang files for project: "/home/travis/build/CloudSlang/cloud-slang-content" failed.
+02/06/17 22:05:30 [ERROR] ---------------
+```
+which file?</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/1004</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>['cloudslang-content-verifier/src/main/java/io/cloudslang/lang/tools/build/verifier/SlangContentVerifier.java']</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>[27, 31, 75, 79, 80, 81, 82, 83, 90, 95, 106, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136]</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/bbb20fab5c5de83d724d3ec3f2c0adf770427078...bb66ee6910987996d31da7be7bf44747ed6200ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>173</v>
+      </c>
+      <c r="E87" t="n">
+        <v>104</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>read_from_file operation context serialization error</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If score tries to create execution message during this operation execution (for example if isRunningTooLong), it fails because  PyFile object, which is serializable  itself ,has field file:TextIOWrapper which is not serializable.
+``` bash
+(SimpleExecutionRunnable.java:126) ERROR - Error during execution!!!
+java.lang.RuntimeException: Failed to serialize execution plan. Error: 
+    at io.cloudslang.engine.queue.entities.ExecutionMessageConverter.objToBytes(ExecutionMessageConverter.java:100)
+    at io.cloudslang.engine.queue.entities.ExecutionMessageConverter.createPayload(ExecutionMessageConverter.java:45)
+    at io.cloudslang.engine.queue.entities.ExecutionMessageConverter.createPayload(ExecutionMessageConverter.java:41)
+    at io.cloudslang.worker.management.services.SimpleExecutionRunnable.createInProgressExecutionMessage(SimpleExecutionRunnable.java:387)
+    at io.cloudslang.worker.management.services.SimpleExecutionRunnable.isRunningTooLong(SimpleExecutionRunnable.java:330)
+    at io.cloudslang.worker.management.services.SimpleExecutionRunnable.shouldStop(SimpleExecutionRunnable.java:175)
+    at io.cloudslang.worker.management.services.SimpleExecutionRunnable.executeRegularStep(SimpleExecutionRunnable.java:161)
+    at io.cloudslang.worker.management.services.SimpleExecutionRunnable.run(SimpleExecutionRunnable.java:119)
+    at java.util.concurrent.Executors$RunnableAdapter.call(Executors.java:511)
+    at java.util.concurrent.FutureTask.run(FutureTask.java:266)
+    at java.util.concurrent.ThreadPoolExecutor.runWorker(ThreadPoolExecutor.java:1142)
+    at java.util.concurrent.ThreadPoolExecutor$Worker.run(ThreadPoolExecutor.java:617)
+    at io.cloudslang.worker.management.services.WorkerThreadFactory$1.run(WorkerThreadFactory.java:33)
+    at java.lang.Thread.run(Thread.java:745)
+Caused by: java.io.NotSerializableException: org.python.core.io.TextIOWrapper
+```
+</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/413</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>['cloudslang-runtime/src/main/java/io/cloudslang/lang/runtime/steps/ActionSteps.java', 'cloudslang-runtime/src/test/java/io/cloudslang/lang/runtime/steps/ActionStepsTest.java']</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>[28, 29, 33, 34, 43, 266, 276, 277, 278, 279, 280, 281, 282, 283, 22, 24, 33, 34, 55, 56, 57, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500]</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/b5d7bcc04c986238d85bf691b32970236d991263...af352cae13eb5354b2059840809ad95564688770</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>173</v>
+      </c>
+      <c r="E88" t="n">
+        <v>104</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Python action - Cannot import svn.local</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When trying to import in an action python script, we get:
+```
+Command failed java.lang.RuntimeException: Slang Error : Error executing python script: Traceback (most recent call last):
+  File "&lt;string&gt;", line 2, in &lt;module&gt;
+  File "C:\\Users\\stoneo\\Desktop\\Cslang-0.8-rc-1\\cslang\\python-lib\\svn\\local.py", line 4, in &lt;module&gt;
+    import svn.common
+  File "C:\\Users\\stoneo\\Desktop\\Cslang-0.8-rc-1\\cslang\\python-lib\\svn\\common.py", line 4, in &lt;module&gt;
+    import dateutil.parser
+  File "C:\\Users\\stoneo\\Desktop\\Cslang-0.8-rc-1\\cslang\\python-lib\\dateutil\\parser.py", line 22, in &lt;module&gt;
+    from io import StringIO
+ImportError: cannot import name StringIO
+```
+If we first import in our script StringIO from io nmaually, it works:
+``` python
+      from io import StringIO
+      import svn.local
+```
+</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/406</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>['cloudslang-runtime/src/test/java/io/cloudslang/lang/runtime/steps/ActionStepsTest.java', 'cloudslang-runtime/src/main/java/io/cloudslang/lang/runtime/configuration/SlangRuntimeSpringConfig.java']</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>[33, 34, 35, 36, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508]</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/031bd28395ebde1bb8817f82daea8a0fe3e51585...564f2613037e39cb8dbcbdfc43abec2adb4817db</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>173</v>
+      </c>
+      <c r="E89" t="n">
+        <v>104</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Double title 'Flow outputs'</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The behavior of the "Flow outputs" messages are changed in CLI. The flow outputs were grouped as a single block. Now we have  'Flow outputs' title for each output:
+E.g.:
+Flow outputs:
+- return_result = Reservation{region=us-east-1, reservationId=r-4cfb859b, instances=[RunningInstance{region=us-east...
+Flow outputs:
+- return_code = 0
+</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/499</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>['cloudslang-cli/src/main/java/io/cloudslang/lang/cli/services/SyncTriggerEventListener.java']</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>[110]</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/956e27184a41ab38ac1d9ddb3c8d2fd1c5705900...fcff612803b0c6d77d499f3a7eb19be3044ae30e</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>173</v>
+      </c>
+      <c r="E90" t="n">
+        <v>104</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Entity references in logs</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some entities still appear as obj refs (e.g. `io.cloudslang.lang.entities.ResultNavigation@5b7d`) instead of toString representation
+</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/510</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>['cloudslang-entities/src/main/java/io/cloudslang/lang/entities/bindings/InOutParam.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/AsyncLoopStatement.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/MapForLoopStatement.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/ListForLoopStatement.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/CompilationArtifact.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/bindings/Input.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/LoopStatement.java', 'cloudslang-entities/src/main/java/io/cloudslang/lang/entities/ResultNavigation.java']</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>['class', 'abstract']</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>[15, 47, 48, 49, 50, 51, 52, 53, 54, 57, 58, 59, 64, 71, 72, 13, 14, 15, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 82, 83, 84, 85, 86, 87, 15, 49, 50, 51, 52, 53, 54, 55, 56, 59, 60, 61, 66, 73, 74, 13, 14, 15, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 15, 57, 58, 59, 60, 61, 62, 63, 64, 65, 68, 69, 70, 75, 83, 84, 14, 46, 47, 48, 49, 50, 51, 52, 53, 56, 57, 58, 63, 64, 70, 75, 49, 50, 51, 52, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 71, 72, 73, 74, 11, 12, 13, 14, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103]</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/4586755a44ef9dde8952ad3bf42c2866a024d651...503644bc56bceca49977883ace69d95586c1c673</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>173</v>
+      </c>
+      <c r="E91" t="n">
+        <v>104</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Sporadic test failures - Travis</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SimpleFlowTest.testFlowWithGlobalSession
+DataFlowTest.testBindingsFlow
+detailed log here: https://gist.github.com/Bonczidai/864f936c36238b5c903b
+</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>https://github.com/CloudSlang/cloud-slang/issues/365</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>['cloudslang-all/src/test/java/io/cloudslang/lang/api/SlangImplTest.java', 'cloudslang-cli/src/main/java/io/cloudslang/lang/cli/SlangCLI.java', 'cloudslang-tests/src/main/java/io/cloudslang/lang/systemtests/TriggerFlows.java', 'cloudslang-content-verifier/src/main/java/io/cloudslang/lang/tools/build/SlangBuildMain.java']</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>['class']</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>[217, 159, 236, 50]</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>https://github.com/cloudslang/cloud-slang/compare/23a53202bd7189b83e508e62679620faf20d22d7...3ad2878242beab856579363dddf16d45fc8db2db</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor bug localization for granular entity selection
Enhanced bug localization to support granular selection and reasoning for files, classes, and functions. Added test file filtering, improved candidate enrichment and consistency logic, and updated LLM prompts for more structured output. Expanded metrics and debugging in evaluation scripts, increased retriever candidate pool, and improved request logging. Minor UI and prompt text changes for clarity.
</commit_message>
<xml_diff>
--- a/Replication Package/Evaluation/test_dataset.xlsx
+++ b/Replication Package/Evaluation/test_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\issue_analyzing_tool\Replication Package\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706C1A2-88BE-4459-9BD2-29A8260B04E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A297D-9D36-413F-AF20-6B29230533AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8955" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2440,12 +2440,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="45.5546875" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
     <col min="9" max="9" width="37.77734375" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
     <col min="11" max="11" width="38.77734375" customWidth="1"/>

</xml_diff>